<commit_message>
Feat commit modul aset
Feat commit modul aset
</commit_message>
<xml_diff>
--- a/cypress/downloads/resultsApproval_Assignmaintenace.xlsx
+++ b/cypress/downloads/resultsApproval_Assignmaintenace.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,7 +421,7 @@
         <v>Pass</v>
       </c>
       <c r="C2" t="str">
-        <v>2025-12-17T07:25:55.293Z</v>
+        <v>2025-12-23T04:56:21.237Z</v>
       </c>
     </row>
     <row r="3">
@@ -432,7 +432,7 @@
         <v>Pass</v>
       </c>
       <c r="C3" t="str">
-        <v>2025-12-17T07:25:55.294Z</v>
+        <v>2025-12-23T04:56:21.238Z</v>
       </c>
     </row>
     <row r="4">
@@ -443,7 +443,7 @@
         <v>Pass</v>
       </c>
       <c r="C4" t="str">
-        <v>2025-12-17T07:25:57.318Z</v>
+        <v>2025-12-23T04:56:21.867Z</v>
       </c>
     </row>
     <row r="5">
@@ -454,7 +454,7 @@
         <v>Pass</v>
       </c>
       <c r="C5" t="str">
-        <v>2025-12-17T07:25:57.598Z</v>
+        <v>2025-12-23T04:56:22.102Z</v>
       </c>
     </row>
     <row r="6">
@@ -465,12 +465,309 @@
         <v>Pass</v>
       </c>
       <c r="C6" t="str">
-        <v>2025-12-17T07:26:12.108Z</v>
+        <v>2025-12-23T04:56:35.863Z</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Company filter option exists: All</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Company filter option exists: PT. BALI TELEKOM</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Company filter option exists: PT. BATAVIA TOWERINDO</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Company filter option exists: PT. INFRASTRUCTURE DIGITAL INDONESIA</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Company filter option exists: PT. JARINGAN PINTAR INDONESIA</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Company filter option exists: PT. MENARA BERSAMA TERPADU</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C12" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Company filter option exists: PT. METRIC SOLUSI INTEGRASI</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C13" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Company filter option exists: PT. MITRAYASA SARANA INFORMASI</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C14" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Company filter option exists: PT. PERMATA KARYA PERDANA</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C15" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Company filter option exists: PT. PRIMA MEDIA SELARAS</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C16" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Company filter option exists: PT. SOLUSINDO KREASI PRATAMA</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C17" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Company filter option exists: PT. SOLUSI MENARA INDONESIA</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C18" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Company filter option exists: PT. TOWER BERSAMA</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C19" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Company filter option exists: PT. TOWER BERSAMA INFRASTRUCTURE</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C20" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Company filter option exists: PT. TELENET INTERNUSA</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C21" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Company filter option exists: PT. TOWERINDO KONVERGENSI</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C22" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Company filter option exists: PT. TOWER ONE</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C23" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Company filter option exists: PT. TRIAKA BERSAMA</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C24" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Company filter option exists: PT. UNITED TOWERINDO</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C25" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Company filter option exists: PT. VISI TELEKOMUNIKASI INFTRASTRUKTUR</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C26" t="str">
+        <v>2025-12-23T04:56:35.904Z</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Button Clicked</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C27" t="str">
+        <v>2025-12-23T04:56:53.523Z</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>User masuk ke Page PV Master List Maintenance</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C28" t="str">
+        <v>2025-12-23T04:56:53.523Z</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>User ID Input</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C29" t="str">
+        <v>2025-12-23T04:56:53.915Z</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Password has been inputed</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C30" t="str">
+        <v>2025-12-23T04:56:54.146Z</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Radio "No" can be clicked via label</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C31" t="str">
+        <v>2025-12-23T04:57:10.300Z</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Search button can be clicked</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C32" t="str">
+        <v>2025-12-23T04:57:10.640Z</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Maintenance table loading spinner disappears</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C33" t="str">
+        <v>2025-12-23T04:57:13.318Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C33"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>